<commit_message>
VAT purchase-sale: formatting update
</commit_message>
<xml_diff>
--- a/VAT Purchase-Sale Excel/Ledger 80-81.xlsx
+++ b/VAT Purchase-Sale Excel/Ledger 80-81.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Stuffs\VAT Purchase-Sale Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8667B0A1-EFD4-41AF-BE18-CADF7C01DB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5973413-ACF9-43BD-85B7-6FF9CD512D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -359,9 +359,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -395,6 +392,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -413,6 +413,146 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle: Diagonal Corners Rounded 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{873EF437-370A-4386-83F8-E9B61F3EC3F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10544174" y="38099"/>
+          <a:ext cx="2000251" cy="1323975"/>
+        </a:xfrm>
+        <a:prstGeom prst="round2DiagRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Make sure the links are OK.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Go to </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>-&gt; Data</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>-&gt; Edit Links</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>-&gt; Change Source</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>And select the correct file.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fPrintsWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1142,7 +1282,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,87 +1292,87 @@
     <col min="5" max="5" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="11" width="13.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.5703125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="str">
+      <c r="A2" s="18" t="str">
         <f>CONCATENATE(_firm," (",_fy1,"-",_fy2,") ",_PAN)</f>
         <v xml:space="preserve"> (2080-2081) </v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
     </row>
     <row r="4" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="20" t="s">
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="19" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1251,13 +1391,13 @@
       <c r="G5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="21"/>
-    </row>
-    <row r="6" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="25"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="20"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>24</v>
       </c>
@@ -1270,7 +1410,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="15"/>
       <c r="J6" s="14"/>
-      <c r="K6" s="17"/>
+      <c r="K6" s="16"/>
       <c r="L6" s="15"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1895,6 +2035,7 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>